<commit_message>
git command file commit 1st
</commit_message>
<xml_diff>
--- a/Git Commands.xlsx
+++ b/Git Commands.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhushanl\Desktop\Bhushan\Knowledge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepository\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0F5AAD-6D74-4086-BD73-632A9E2583CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95B4033-07A3-4470-9F5F-45BB043A238B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Description</t>
   </si>
@@ -266,6 +266,51 @@
   </si>
   <si>
     <t>$ git diff &lt;source commit id &gt; &lt;destination commit id &gt; &lt;file name&gt;</t>
+  </si>
+  <si>
+    <t>git rm</t>
+  </si>
+  <si>
+    <t>It will remove all files</t>
+  </si>
+  <si>
+    <t>$ git rm -r .</t>
+  </si>
+  <si>
+    <t>$ git rm &lt;file name&gt;</t>
+  </si>
+  <si>
+    <t>To Remove Files Only from staging Area not from working directory(git rm --cached)</t>
+  </si>
+  <si>
+    <t>$ git rm --cached &lt;file name&gt;</t>
+  </si>
+  <si>
+    <t>To Remove Files Only from Working Directory (rm Command)</t>
+  </si>
+  <si>
+    <t>$ rm &lt;file name&gt;</t>
+  </si>
+  <si>
+    <t>To Remove Files from both  Working Directory and staging Area (git rm)                                                        Note: for git rm command argument is mandatory</t>
+  </si>
+  <si>
+    <t>$ git checkout -- &lt;filename&gt;</t>
+  </si>
+  <si>
+    <t>git checkout</t>
+  </si>
+  <si>
+    <t>$ git checkout</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>We can use checkout command to discard(undo) unstaged changes in the tracked files of working directory. To discard unstaged changes(The changes which are not added to staging area). It will discard any unstaged changes made in file. After executing this command, staged copy content and working directory content is same.</t>
+  </si>
+  <si>
+    <t>To discard changes in all tracked files of working directory.(The files which are already added to staging area/commit).If we are not passing any argument, then this command will show the list of eligible files for checkout.                                                                                                                     Note: git checkout command can be used in branching also.</t>
   </si>
 </sst>
 </file>
@@ -374,13 +419,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -394,23 +455,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,16 +741,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D40"/>
+  <dimension ref="A2:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" style="1" customWidth="1"/>
     <col min="3" max="3" width="84.08984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="91.54296875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="1"/>
@@ -708,13 +758,13 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -747,13 +797,13 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -761,26 +811,26 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -790,7 +840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="2" t="s">
@@ -801,10 +851,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -815,8 +865,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
@@ -825,18 +875,18 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
@@ -845,19 +895,19 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -865,9 +915,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -875,9 +925,9 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -885,22 +935,22 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -922,13 +972,13 @@
       <c r="A21" s="2">
         <v>7</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -936,42 +986,42 @@
       <c r="A22" s="2">
         <v>8</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>9</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -979,9 +1029,9 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="11" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -989,8 +1039,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="2" t="s">
         <v>56</v>
       </c>
@@ -999,19 +1049,19 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="9" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="9" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D29" s="13" t="s">
@@ -1019,79 +1069,112 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="11" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="9" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="9" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" t="s">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+    <row r="34" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="6">
+        <v>10</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A38" s="6">
+        <v>11</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A39" s="8"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
@@ -1099,8 +1182,17 @@
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C41" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A38:A39"/>
     <mergeCell ref="A10:A19"/>
     <mergeCell ref="B23:B33"/>
     <mergeCell ref="A23:A33"/>

</xml_diff>

<commit_message>
Git repo commit 2nd
</commit_message>
<xml_diff>
--- a/Git Commands.xlsx
+++ b/Git Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepository\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95B4033-07A3-4470-9F5F-45BB043A238B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05F49A4-0622-4D19-94E8-137D9618856C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
   <si>
     <t>Description</t>
   </si>
@@ -304,13 +304,140 @@
     <t>$ git checkout</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>We can use checkout command to discard(undo) unstaged changes in the tracked files of working directory. To discard unstaged changes(The changes which are not added to staging area). It will discard any unstaged changes made in file. After executing this command, staged copy content and working directory content is same.</t>
   </si>
   <si>
-    <t>To discard changes in all tracked files of working directory.(The files which are already added to staging area/commit).If we are not passing any argument, then this command will show the list of eligible files for checkout.                                                                                                                     Note: git checkout command can be used in branching also.</t>
+    <t>$ git config --global alias.&lt;aliasname&gt; "&lt;original command without git&gt;"  Ex. git config --global alias.one "log --oneline"</t>
+  </si>
+  <si>
+    <t>We can create alias name by using git config command.                                                                 Note: After creating alias name, we can use either alias name or original name.</t>
+  </si>
+  <si>
+    <t>git touch</t>
+  </si>
+  <si>
+    <t>It is very common requirement that we are not required to store everything in the repository.Ignoring unwanted Files and  Directories by using .gitignore File. Insert files name in this file to ignore that files</t>
+  </si>
+  <si>
+    <t>$ git branch</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>To create a new branch by using git branch command.</t>
+  </si>
+  <si>
+    <t>To Switch from one Branch to another Branch .We have to use git checkout command. We used git checkout command already to discard unstaged changes in working directory.</t>
+  </si>
+  <si>
+    <t>Shortcut command to Create a New Branch and switch to that Branch.We have to use -b option with checkout command</t>
+  </si>
+  <si>
+    <t>$ git branch &lt;new branch name&gt;</t>
+  </si>
+  <si>
+    <t>$ git checkout -b &lt;new branch name&gt;</t>
+  </si>
+  <si>
+    <t>$ git checkout &lt;branch name on switch&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To know all available branches in our local repository, we have to use git branch command.                             - By default we have only one branch: master . * indicates that master is current active branch.                                                                                                          Note: There is another way to check on which branch currently we are working, for this we have 
+to use git status command. . Once we creates a branch all files and commits will be inherited from parent branch to child branch. Branching is a logical way of duplicating files and commits. For every branch, new directory won't be created. </t>
+  </si>
+  <si>
+    <t>To discard changes in all tracked files of working directory.(The files which are already added to staging area/commit).If we are not passing any argument, then this command will show the list of eligible files for checkout.                                                                                                                              Note: git checkout command can be used in branching also.</t>
+  </si>
+  <si>
+    <t>$ git merge &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>git merge</t>
+  </si>
+  <si>
+    <t>$ touch .gitignore  (To create file)                                                                                                                                        Ex add.# Don't track abc.txt file
+abc.txt
+# Don't track all .txt files
+*.txt
+# Don't track logs directory
+logs/
+#Don't track any hidden file
+.*</t>
+  </si>
+  <si>
+    <t>To create new files and add them to the index in a Git repository. This command simplifies the process of tracking new files and ensures they are included in the next commit.                              This command takes one or more file paths as arguments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ git touch &lt;file name&gt; or  $ git touch &lt;folder name&gt;/&lt;file name&gt; (If in specific forlder)                                                                                                                                                       $git touch &lt;folder name&gt;/&lt;file name&gt;   &lt;folder name&gt;/&lt;file name&gt;                                                                                                                                                                 </t>
+  </si>
+  <si>
+    <r>
+      <t>We can perform merge operation by using git merge command.                                                          We have to execute this command from parent branch. After creating child branch, if we are not doing any new commits in the parent branch,  then git will perform</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fast-forward merge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. i.e updations(new commits) happened only in child branch but not in parent branch. thats why no confilct will be raised.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If changes present in both parent and child branches and if we are trying to perform 
+merge operation, then git will do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>three-way merge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.Three-way merge creates a new commit which is also known as merge commit.
+Parent branch will pointing to the newly created merge commit.In the case of 3-way merge, if the same file updated by both Parent and child branches then may be a chance of merge conflict.We have to resolve the conflict manually by editing the file.</t>
+    </r>
+  </si>
+  <si>
+    <t>To delete a branch by using git branch command with -d option.Deletion of the branch is optional. After deleting the branch, still files and commits are available because the changes are 
+merged to master branch.</t>
+  </si>
+  <si>
+    <t>$ git branch -d &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>If we want to combine all commits of xyz branch into a single commit and merge that 
+commit to the master branch, then we should go for squash option.</t>
+  </si>
+  <si>
+    <t>$ git merge --squash &lt;branch name&gt;</t>
   </si>
 </sst>
 </file>
@@ -419,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -434,6 +561,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -444,7 +574,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -455,11 +585,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,467 +877,653 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D41"/>
+  <dimension ref="B2:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="84.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="91.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="81.6328125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="91.54296875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="2"/>
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+    <row r="3" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+    <row r="4" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
+    <row r="5" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="2" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="2" t="s">
+    <row r="7" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+    <row r="8" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="2" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+    <row r="10" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="2" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="4" t="s">
+    <row r="12" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="2" t="s">
+    <row r="13" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="4" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="4" t="s">
+    <row r="16" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="4" t="s">
+    <row r="17" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="4" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="4" t="s">
+    <row r="19" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+    <row r="20" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B20" s="7">
         <v>6</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+    <row r="21" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="2">
         <v>7</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D22" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="2">
         <v>8</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D23" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
+    <row r="24" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="7">
         <v>9</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="4" t="s">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="4" t="s">
+    <row r="26" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="4" t="s">
+    <row r="27" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="2" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="4" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="4" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="E30" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="4" t="s">
+    <row r="31" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="4" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="4" t="s">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="4" t="s">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="6">
+    <row r="35" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="7">
         <v>10</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D35" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="4" t="s">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E36" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="4" t="s">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="E37" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="4" t="s">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E38" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A38" s="6">
+    <row r="39" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="B39" s="10">
         <v>11</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="C39" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A39" s="8"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="2" t="s">
+    <row r="40" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C41" s="1" t="s">
-        <v>83</v>
-      </c>
+    <row r="41" spans="2:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B41" s="7">
+        <v>12</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B43" s="7">
+        <v>13</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" s="8"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B45" s="8"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B47" s="7">
+        <v>14</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A10:A19"/>
-    <mergeCell ref="B23:B33"/>
-    <mergeCell ref="A23:A33"/>
+  <mergeCells count="21">
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="D5:D7"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="B10:B19"/>
+    <mergeCell ref="C24:C34"/>
+    <mergeCell ref="B24:B34"/>
+    <mergeCell ref="C10:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Git command commit 3rd
</commit_message>
<xml_diff>
--- a/Git Commands.xlsx
+++ b/Git Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepository\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05F49A4-0622-4D19-94E8-137D9618856C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9024F682-5753-4A3C-9597-032E2CAE73DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="136">
   <si>
     <t>Description</t>
   </si>
@@ -438,6 +438,114 @@
   </si>
   <si>
     <t>$ git merge --squash &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>git reset</t>
+  </si>
+  <si>
+    <t>$ git reset &lt;file name&gt;</t>
+  </si>
+  <si>
+    <t>We can use git reset to remove changes from staging area.
+Changes already added to staging area, but if we don't want to commit, then to remove 
+such type of changes from staging area, then we should go for git reset.
+It will bring the changes from staging area back to working directory.In reset file won't be removed from staging area, but reset to previous state(one step back).</t>
+  </si>
+  <si>
+    <t>$ git reset &lt;mode&gt; &lt;commit id&gt;</t>
+  </si>
+  <si>
+    <t>We can also use reset to undo commits at repository level .Moves the HEAD to the specified commit, and all remaining recent commits will be  removed. mode will decide whether these changes are going to remove from staging area and working directory or not.                                  The allowed values for the mode are:
+ --mixed
+ --soft
+ --hard
+ --keep
+ --merge</t>
+  </si>
+  <si>
+    <t>$ git reset --mixed &lt;commit id&gt;
+$ git reset --mixed HEAD~1 (remove last commit)
+$ git reset HEAD~1</t>
+  </si>
+  <si>
+    <t>mixed Mode -It is the default mode.To discard commits in the local repository and to discard changes in staging area we should use reset with --mixed option.It won't touch working directory. Note: 
+1) It is not possible to remove random commits.
+2) --mixed will work only on repository and staging area but not on working directory.</t>
+  </si>
+  <si>
+    <t>$ git reset --soft &lt;commit id&gt;</t>
+  </si>
+  <si>
+    <t>Reset with --hard :It is exactly same as --mixed except that Changes will be removed from everywhere (local repository,staging area,working directory)
+It is more dangerous command and it is destructive command.
+It is impossible to revert back and hence while using hard reset we have to take special care</t>
+  </si>
+  <si>
+    <t>$ git reset --hard &lt;commit id&gt;</t>
+  </si>
+  <si>
+    <t>soft mode - It is exactly same as --mixed option, Changes will be discarded only in local repository.
+As changes already present in staging area, just we have to use commit to revert back.The commits will be discarded only in local repository, but changes will be there in working directory and staging area.To Revert Changes we have to do Just  git commit -m "&lt;message&gt;"</t>
+  </si>
+  <si>
+    <t>Note: If the commits are confirmed to local repository and to discard those commits we can use 
+reset command.not recommend on remote repository</t>
+  </si>
+  <si>
+    <t>git rebase</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>git stash</t>
+  </si>
+  <si>
+    <t>$ git stash</t>
+  </si>
+  <si>
+    <t>Rebase is alternative way to merge changes of two branches togther.
+rebase = re + base =&gt; re arrange base</t>
+  </si>
+  <si>
+    <t>The git stash command takes our uncommitted changes (both staged and unstaged), saves 
+in some temporary location.
+After completing our urgent work, we can bring these stashed changes to our current working directory.                                                                                                                                                       Note: 1. Stashing concept is applicable only for tracked files but not for newly created files. 
+2. To perform stashing, atleast one commit must be completed.  Assume we required to create and work on file3.txt and and this file changes needs to be 
+committed immediately.To work on file3.txt, we have to save uncommitted changes of file1.txt and file2.txt to some temporary location, because we don't want to include these changes in the current commit. For this we should go for git stash command.</t>
+  </si>
+  <si>
+    <t>$ git stash list</t>
+  </si>
+  <si>
+    <t>To check the contents of stash</t>
+  </si>
+  <si>
+    <t>To list all available stashes</t>
+  </si>
+  <si>
+    <t>$ git show stash@{0}</t>
+  </si>
+  <si>
+    <t>We have to bring files from temporary location to our working directory. For this we have 
+to perform unstash operation.We can perform unstashing in 2 ways:
+1. by using git stash pop
+2. by using git stash apply</t>
+  </si>
+  <si>
+    <t>By using git stash pop:
+It will bring stashed changes from temporary location to working directory.
+The corresponding entry will be deleted.</t>
+  </si>
+  <si>
+    <t>$ git stash pop stash@{0}</t>
+  </si>
+  <si>
+    <t>By using git stash apply:
+It will bring stashed changes from temporary location to working directory.But, the corresponding entry won't be deleted, so that we can use this stash in other branches to continue their work.</t>
+  </si>
+  <si>
+    <t>$ git stash apply stash@{0}</t>
   </si>
 </sst>
 </file>
@@ -546,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -564,18 +672,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -584,18 +713,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -877,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E61"/>
+  <dimension ref="B2:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -888,7 +1005,7 @@
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="5" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="81.6328125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="81.6328125" style="9" customWidth="1"/>
     <col min="5" max="5" width="91.54296875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
@@ -898,7 +1015,7 @@
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -912,7 +1029,7 @@
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -926,7 +1043,7 @@
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -934,13 +1051,13 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="11">
+      <c r="B5" s="18">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -948,29 +1065,29 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="16"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="16"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="7">
+      <c r="B8" s="13">
         <v>4</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -978,9 +1095,9 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="15" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -988,13 +1105,13 @@
       </c>
     </row>
     <row r="10" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="7">
+      <c r="B10" s="13">
         <v>5</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1002,9 +1119,9 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="15" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1012,9 +1129,9 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="15" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1022,9 +1139,9 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="15" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1032,9 +1149,9 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="15" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1042,9 +1159,9 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="15" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -1052,9 +1169,9 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="15" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1062,9 +1179,9 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="15" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1072,9 +1189,9 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="15" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -1082,9 +1199,9 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="15" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -1092,13 +1209,13 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="B20" s="7">
+      <c r="B20" s="13">
         <v>6</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1106,9 +1223,9 @@
       </c>
     </row>
     <row r="21" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="17" t="s">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="9" t="s">
         <v>85</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -1122,7 +1239,7 @@
       <c r="C22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -1136,7 +1253,7 @@
       <c r="C23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -1144,21 +1261,21 @@
       </c>
     </row>
     <row r="24" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B24" s="7">
+      <c r="B24" s="13">
         <v>9</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="8" t="s">
         <v>52</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="15" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="8" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -1166,9 +1283,9 @@
       </c>
     </row>
     <row r="26" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="15" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="8" t="s">
         <v>54</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -1176,9 +1293,9 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="15" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="8" t="s">
         <v>55</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -1186,9 +1303,9 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="15" t="s">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="8" t="s">
         <v>56</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -1196,9 +1313,9 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="15" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -1206,9 +1323,9 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="15" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="8" t="s">
         <v>60</v>
       </c>
       <c r="E30" s="6" t="s">
@@ -1216,9 +1333,9 @@
       </c>
     </row>
     <row r="31" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="15" t="s">
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -1226,9 +1343,9 @@
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="15" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="8" t="s">
         <v>63</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -1236,9 +1353,9 @@
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="15" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -1246,9 +1363,9 @@
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="15" t="s">
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -1256,13 +1373,13 @@
       </c>
     </row>
     <row r="35" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B35" s="7">
+      <c r="B35" s="13">
         <v>10</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="8" t="s">
         <v>79</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -1270,9 +1387,9 @@
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="15" t="s">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -1280,9 +1397,9 @@
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="15" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="8" t="s">
         <v>75</v>
       </c>
       <c r="E37" s="4" t="s">
@@ -1290,9 +1407,9 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="15" t="s">
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -1300,13 +1417,13 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B39" s="10">
+      <c r="B39" s="16">
         <v>11</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="8" t="s">
         <v>83</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -1314,9 +1431,9 @@
       </c>
     </row>
     <row r="40" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="15" t="s">
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="8" t="s">
         <v>97</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -1324,13 +1441,13 @@
       </c>
     </row>
     <row r="41" spans="2:5" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="7">
+      <c r="B41" s="13">
         <v>12</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="8" t="s">
         <v>87</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -1338,9 +1455,9 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="15" t="s">
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="8" t="s">
         <v>101</v>
       </c>
       <c r="E42" s="2" t="s">
@@ -1348,13 +1465,13 @@
       </c>
     </row>
     <row r="43" spans="2:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="B43" s="7">
+      <c r="B43" s="13">
         <v>13</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="8" t="s">
         <v>96</v>
       </c>
       <c r="E43" s="4" t="s">
@@ -1362,9 +1479,9 @@
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B44" s="8"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="15" t="s">
+      <c r="B44" s="14"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="8" t="s">
         <v>90</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1372,9 +1489,9 @@
       </c>
     </row>
     <row r="45" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B45" s="8"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="15" t="s">
+      <c r="B45" s="14"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1382,138 +1499,243 @@
       </c>
     </row>
     <row r="46" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="15" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="8" t="s">
         <v>92</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B47" s="7">
+    <row r="47" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B47" s="11"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B48" s="13">
         <v>14</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C48" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D48" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="15" t="s">
-        <v>104</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>106</v>
+    <row r="49" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="15" t="s">
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="8" t="s">
         <v>107</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="15"/>
+    <row r="51" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B51" s="13">
+        <v>15</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="12" t="s">
+        <v>120</v>
+      </c>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="2"/>
+    <row r="57" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B57" s="2">
+        <v>16</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="B58" s="13">
+        <v>17</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="2"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="15"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="E61" s="2"/>
     </row>
+    <row r="62" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
+  <mergeCells count="25">
+    <mergeCell ref="C58:C63"/>
+    <mergeCell ref="B58:B63"/>
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="C39:C40"/>
@@ -1524,7 +1746,21 @@
     <mergeCell ref="C10:C19"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C51:C56"/>
+    <mergeCell ref="B51:B56"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
git command commit 4th
</commit_message>
<xml_diff>
--- a/Git Commands.xlsx
+++ b/Git Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepository\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9024F682-5753-4A3C-9597-032E2CAE73DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C23371-23F2-4D59-BF07-D73721C61EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
   <si>
     <t>Description</t>
   </si>
@@ -546,6 +546,99 @@
   </si>
   <si>
     <t>$ git stash apply stash@{0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can perform partial stash by using the following command: $ git stash -p                                     Assume we have multiple files, but we want stash only for some files. It is possible and 
+this concept is called partial stash. </t>
+  </si>
+  <si>
+    <t>$ git stash -p</t>
+  </si>
+  <si>
+    <t>To delete all the stashes</t>
+  </si>
+  <si>
+    <t>$ git stash clear</t>
+  </si>
+  <si>
+    <t>$ git stash drop &lt;stash id&gt;</t>
+  </si>
+  <si>
+    <t>To delete a particular stash</t>
+  </si>
+  <si>
+    <t>git remote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can use git remote command to configure remote repository to our local repository. </t>
+  </si>
+  <si>
+    <t>$ git remote add &lt;alias_name to remote repo url&gt; &lt;remote_repository_url&gt;</t>
+  </si>
+  <si>
+    <t>$ git remote</t>
+  </si>
+  <si>
+    <t>To see all alias names of remote repositories</t>
+  </si>
+  <si>
+    <t>To see all alias names and url of remote repositories</t>
+  </si>
+  <si>
+    <t>$ git remote -v</t>
+  </si>
+  <si>
+    <t>$ git push &lt;remote_name&gt; &lt;branch_name&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can use git push command to send our changes from local repository to remote 
+repository. ie to push our changes from local repo to remote repo. </t>
+  </si>
+  <si>
+    <t>git clone</t>
+  </si>
+  <si>
+    <t>cloning or duplicating exact copy remote repository to local repository.
+Already there is a project on remote repository.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $ git clone &lt;remote_repo_url&gt;</t>
+  </si>
+  <si>
+    <t>Based on our requirement we can provide a new name for the project.</t>
+  </si>
+  <si>
+    <t>$ git clone &lt;remote_repo_url&gt;  &lt;new_project_name&gt;</t>
+  </si>
+  <si>
+    <t>We can use get fetch command to check whether any updates available at remote 
+repository or not. This command will retrieve only latest meta-data info from the remote 
+repository. It won't download updates from remote repository into local repository.</t>
+  </si>
+  <si>
+    <t>git fetch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $ git fetch &lt;remote_repo_name&gt;</t>
+  </si>
+  <si>
+    <t>git pull</t>
+  </si>
+  <si>
+    <t>$ git pull &lt;remote_repo_name&gt; &lt;branch name&gt;</t>
+  </si>
+  <si>
+    <t>We can use git pull command to download and merge updates from remote repository 
+into local repository.                                                                                                                                                  Note: To perform push operation, local repository and remote repository should be in sync. ie 
+the local repository should be upto date to the remote repository.If any updates in remote repo, git push is not allowed. It will ask us to pull first.</t>
+  </si>
+  <si>
+    <t>Tag is nothing but a label or mark to a particular commit in our repository.
+Tag is static and permanent reference to a particular commit where as HEAD/Branch is a 
+dynamic reference.In general Tags can be used for release verions</t>
+  </si>
+  <si>
+    <t>git tag</t>
   </si>
 </sst>
 </file>
@@ -654,7 +747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -713,6 +806,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E70"/>
+  <dimension ref="B2:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1005,7 +1110,7 @@
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="5" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="81.6328125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="84.90625" style="9" customWidth="1"/>
     <col min="5" max="5" width="91.54296875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
@@ -1236,7 +1341,7 @@
       <c r="B22" s="2">
         <v>7</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="8" t="s">
@@ -1250,7 +1355,7 @@
       <c r="B23" s="2">
         <v>8</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="21" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="8" t="s">
@@ -1282,7 +1387,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="8" t="s">
@@ -1586,7 +1691,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="8" t="s">
@@ -1629,10 +1734,10 @@
       </c>
     </row>
     <row r="58" spans="2:5" ht="145" x14ac:dyDescent="0.35">
-      <c r="B58" s="13">
+      <c r="B58" s="16">
         <v>17</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="16" t="s">
         <v>123</v>
       </c>
       <c r="D58" s="8" t="s">
@@ -1643,8 +1748,8 @@
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
       <c r="D59" s="3" t="s">
         <v>129</v>
       </c>
@@ -1653,8 +1758,8 @@
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
       <c r="D60" s="8" t="s">
         <v>128</v>
       </c>
@@ -1663,16 +1768,16 @@
       </c>
     </row>
     <row r="61" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
       <c r="D61" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E61" s="2"/>
     </row>
     <row r="62" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="8" t="s">
         <v>132</v>
       </c>
@@ -1681,8 +1786,8 @@
       </c>
     </row>
     <row r="63" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
       <c r="D63" s="8" t="s">
         <v>134</v>
       </c>
@@ -1690,67 +1795,219 @@
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="2"/>
+    <row r="64" spans="2:5" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="2"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="2"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="2"/>
+      <c r="B67" s="13">
+        <v>18</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="2"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="2"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B70" s="15"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B71" s="13">
+        <v>19</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B73" s="2">
+        <v>20</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B74" s="2">
+        <v>21</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B75" s="2">
+        <v>22</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="C58:C63"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="B39:B40"/>
+  <mergeCells count="29">
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B19"/>
     <mergeCell ref="C24:C34"/>
     <mergeCell ref="B24:B34"/>
     <mergeCell ref="C10:C19"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="C51:C56"/>
     <mergeCell ref="B51:B56"/>
     <mergeCell ref="C43:C46"/>
@@ -1759,6 +2016,8 @@
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="C48:C50"/>
     <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="B58:B66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
Git commnad file commit 5th
</commit_message>
<xml_diff>
--- a/Git Commands.xlsx
+++ b/Git Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepository\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C23371-23F2-4D59-BF07-D73721C61EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0840D605-67C9-45DC-9DFA-C1312E97DF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="194">
   <si>
     <t>Description</t>
   </si>
@@ -633,12 +633,110 @@
 the local repository should be upto date to the remote repository.If any updates in remote repo, git push is not allowed. It will ask us to pull first.</t>
   </si>
   <si>
+    <t>git tag</t>
+  </si>
+  <si>
+    <t>Creation of a Light Weight Tag ,We have to use git tag command.</t>
+  </si>
+  <si>
+    <t>$ git tag &lt;tag_name&gt;</t>
+  </si>
+  <si>
+    <t>We can list available tags by using -l or --list option</t>
+  </si>
+  <si>
+    <t>$ git tab -l or $ git tab --list</t>
+  </si>
+  <si>
+    <t>We can use tag directly where ever commit id is required in our commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ git show &lt;commitid&gt; </t>
+  </si>
+  <si>
+    <t>$ git show &lt;tagname&gt;</t>
+  </si>
+  <si>
+    <t>For the specified commitid, if any tag is defined then we can use directly that tag instead 
+of commit id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To delete  use git tag command with -d or --delete option.</t>
+  </si>
+  <si>
+    <t>$ git tag -d &lt;tagname&gt;</t>
+  </si>
+  <si>
     <t>Tag is nothing but a label or mark to a particular commit in our repository.
 Tag is static and permanent reference to a particular commit where as HEAD/Branch is a 
-dynamic reference.In general Tags can be used for release verions</t>
-  </si>
-  <si>
-    <t>git tag</t>
+dynamic reference.In general Tags can be used for release verions. The tags will be stored in our repository inside tags folder(.git/refs/tags).    There are two types of tags :
+1) Light Weight/Simple Tags
+2) Annotated Tags [Tags with Information]                                                                                                          Note: Within the repository, tag name should be unique.</t>
+  </si>
+  <si>
+    <t>Annotated Tag is exactly same as Light weight tag except that it maintains information like 
+tagger name, date of creation, description etc.Annotated Tag internally maintained as object form in git repository. Annotated tags will be stored in .git/refs/tags folder and .git/objects folder.</t>
+  </si>
+  <si>
+    <t>To create annotated tag by using git tag command with -a option.</t>
+  </si>
+  <si>
+    <t>$ git tag -a &lt;tagname&gt; &amp; $ git tag -a &lt;tagname&gt; -m &lt;tag_message&gt;</t>
+  </si>
+  <si>
+    <t>$ git tag -a &lt;tagname&gt; &lt;commitid&gt; -m &lt;tagmessage&gt;</t>
+  </si>
+  <si>
+    <t>To Tag a previous particular Commit</t>
+  </si>
+  <si>
+    <t>$ git tag -a &lt;tagname&gt; -f &lt;newcommitid&gt; -m &lt;tagmessage&gt;</t>
+  </si>
+  <si>
+    <t>To update an existing Tag .It is possible to update the tag to the correct commit.
+We can do this by using the following 2 ways.
+1) Delete the tag and Recreate tag with corresponding correct commit id.
+2) By using -f or --force option to replace an existing tag without deleting.                                                Note: For the same commit we can define multiple tags also based on our requirement. Is it not Possible to use same Tag for multiple Commits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To compare two Tags. We can use difftool command also.
+</t>
+  </si>
+  <si>
+    <t>$ git diff &lt;tag one&gt; &lt;tag two&gt; or  $ git difftool  &lt;tag one&gt; &lt;tag two&gt;</t>
+  </si>
+  <si>
+    <t>To Push Tags to remote Repository.Bydefault push command wont push tags to the remote repository. We have to push tags separately. To push a Single Tag use command</t>
+  </si>
+  <si>
+    <t>$ git push &lt;repository name&gt; &lt;tagname&gt;</t>
+  </si>
+  <si>
+    <t>$ git push &lt;repository name&gt; &lt;branch name&gt; --tags</t>
+  </si>
+  <si>
+    <t>We have to use --tags option with git push command to push all Tags at remote repo.</t>
+  </si>
+  <si>
+    <t>$ git push &lt;repository name&gt; : &lt;tag name&gt;</t>
+  </si>
+  <si>
+    <t>To delete a Tag from the Remote Repository.the tag will be deleted from the remote repository, but not from local repository.</t>
+  </si>
+  <si>
+    <t>git revert</t>
+  </si>
+  <si>
+    <t>$ git revert &lt;commit id&gt;</t>
+  </si>
+  <si>
+    <t>git revert command won't delete commit history. It reverts / undo the required commit by creating a new commit. i.e it will undo a particular commit without deleting commit history.git reset command deletes commit history.In git revert, commit history won't be deleted and hence there is no effect on peer developers. Note: We can revert any commit, need not be last commit.When you revert a commit c then all the commits made after c will also get reverted.</t>
+  </si>
+  <si>
+    <t>$ git revert --no-commit &lt;commit id&gt;</t>
+  </si>
+  <si>
+    <t>git revert command adds a new commit by default.-n or --no-commit flag will applies the revert  to your working directory and staging area but doesn't create a new commit. It allows you to make further modifications or additions before committing the reversion.</t>
   </si>
 </sst>
 </file>
@@ -783,6 +881,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -792,8 +893,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -808,16 +915,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1099,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E84"/>
+  <dimension ref="B2:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1110,7 +1208,7 @@
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="5" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="84.90625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="85.90625" style="9" customWidth="1"/>
     <col min="5" max="5" width="91.54296875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
@@ -1156,13 +1254,13 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="18">
+      <c r="B5" s="21">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1170,26 +1268,26 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="17"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="17"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="13">
+      <c r="B8" s="14">
         <v>4</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -1200,8 +1298,8 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
@@ -1210,10 +1308,10 @@
       </c>
     </row>
     <row r="10" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="13">
+      <c r="B10" s="14">
         <v>5</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -1224,8 +1322,8 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="8" t="s">
         <v>31</v>
       </c>
@@ -1234,8 +1332,8 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="8" t="s">
         <v>33</v>
       </c>
@@ -1244,8 +1342,8 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="8" t="s">
         <v>34</v>
       </c>
@@ -1254,8 +1352,8 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="8" t="s">
         <v>35</v>
       </c>
@@ -1264,8 +1362,8 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="8" t="s">
         <v>38</v>
       </c>
@@ -1274,8 +1372,8 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="8" t="s">
         <v>40</v>
       </c>
@@ -1284,8 +1382,8 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="8" t="s">
         <v>42</v>
       </c>
@@ -1294,8 +1392,8 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="8" t="s">
         <v>44</v>
       </c>
@@ -1304,8 +1402,8 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="8" t="s">
         <v>47</v>
       </c>
@@ -1314,10 +1412,10 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="B20" s="13">
+      <c r="B20" s="14">
         <v>6</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -1328,8 +1426,8 @@
       </c>
     </row>
     <row r="21" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="9" t="s">
         <v>85</v>
       </c>
@@ -1341,7 +1439,7 @@
       <c r="B22" s="2">
         <v>7</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="8" t="s">
@@ -1355,7 +1453,7 @@
       <c r="B23" s="2">
         <v>8</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="8" t="s">
@@ -1366,10 +1464,10 @@
       </c>
     </row>
     <row r="24" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B24" s="13">
+      <c r="B24" s="14">
         <v>9</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -1378,8 +1476,8 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="8" t="s">
         <v>50</v>
       </c>
@@ -1388,8 +1486,8 @@
       </c>
     </row>
     <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="8" t="s">
         <v>54</v>
       </c>
@@ -1398,8 +1496,8 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="8" t="s">
         <v>55</v>
       </c>
@@ -1408,8 +1506,8 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="8" t="s">
         <v>56</v>
       </c>
@@ -1418,8 +1516,8 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="8" t="s">
         <v>58</v>
       </c>
@@ -1428,8 +1526,8 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="8" t="s">
         <v>60</v>
       </c>
@@ -1438,8 +1536,8 @@
       </c>
     </row>
     <row r="31" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="8" t="s">
         <v>61</v>
       </c>
@@ -1448,8 +1546,8 @@
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="8" t="s">
         <v>63</v>
       </c>
@@ -1458,8 +1556,8 @@
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="8" t="s">
         <v>65</v>
       </c>
@@ -1468,8 +1566,8 @@
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="8" t="s">
         <v>66</v>
       </c>
@@ -1478,10 +1576,10 @@
       </c>
     </row>
     <row r="35" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B35" s="13">
+      <c r="B35" s="14">
         <v>10</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="14" t="s">
         <v>71</v>
       </c>
       <c r="D35" s="8" t="s">
@@ -1492,8 +1590,8 @@
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="8" t="s">
         <v>72</v>
       </c>
@@ -1502,8 +1600,8 @@
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="8" t="s">
         <v>75</v>
       </c>
@@ -1512,8 +1610,8 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="8" t="s">
         <v>77</v>
       </c>
@@ -1522,10 +1620,10 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B39" s="16">
+      <c r="B39" s="24">
         <v>11</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="24" t="s">
         <v>81</v>
       </c>
       <c r="D39" s="8" t="s">
@@ -1536,8 +1634,8 @@
       </c>
     </row>
     <row r="40" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="8" t="s">
         <v>97</v>
       </c>
@@ -1546,10 +1644,10 @@
       </c>
     </row>
     <row r="41" spans="2:5" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="13">
+      <c r="B41" s="14">
         <v>12</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="14" t="s">
         <v>86</v>
       </c>
       <c r="D41" s="8" t="s">
@@ -1560,8 +1658,8 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="8" t="s">
         <v>101</v>
       </c>
@@ -1570,10 +1668,10 @@
       </c>
     </row>
     <row r="43" spans="2:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="B43" s="13">
+      <c r="B43" s="14">
         <v>13</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="24" t="s">
         <v>89</v>
       </c>
       <c r="D43" s="8" t="s">
@@ -1584,8 +1682,8 @@
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B44" s="14"/>
-      <c r="C44" s="16"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="24"/>
       <c r="D44" s="8" t="s">
         <v>90</v>
       </c>
@@ -1594,8 +1692,8 @@
       </c>
     </row>
     <row r="45" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B45" s="14"/>
-      <c r="C45" s="16"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="8" t="s">
         <v>91</v>
       </c>
@@ -1604,8 +1702,8 @@
       </c>
     </row>
     <row r="46" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B46" s="15"/>
-      <c r="C46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="24"/>
       <c r="D46" s="8" t="s">
         <v>92</v>
       </c>
@@ -1624,10 +1722,10 @@
       </c>
     </row>
     <row r="48" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B48" s="13">
+      <c r="B48" s="14">
         <v>14</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="14" t="s">
         <v>99</v>
       </c>
       <c r="D48" s="8" t="s">
@@ -1638,8 +1736,8 @@
       </c>
     </row>
     <row r="49" spans="2:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
       <c r="D49" s="8" t="s">
         <v>104</v>
       </c>
@@ -1648,8 +1746,8 @@
       </c>
     </row>
     <row r="50" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="8" t="s">
         <v>107</v>
       </c>
@@ -1658,10 +1756,10 @@
       </c>
     </row>
     <row r="51" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B51" s="13">
+      <c r="B51" s="14">
         <v>15</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="14" t="s">
         <v>109</v>
       </c>
       <c r="D51" s="8" t="s">
@@ -1672,8 +1770,8 @@
       </c>
     </row>
     <row r="52" spans="2:5" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
       <c r="D52" s="12" t="s">
         <v>113</v>
       </c>
@@ -1682,8 +1780,8 @@
       </c>
     </row>
     <row r="53" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
       <c r="D53" s="8" t="s">
         <v>115</v>
       </c>
@@ -1692,8 +1790,8 @@
       </c>
     </row>
     <row r="54" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
       <c r="D54" s="8" t="s">
         <v>119</v>
       </c>
@@ -1702,8 +1800,8 @@
       </c>
     </row>
     <row r="55" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
       <c r="D55" s="8" t="s">
         <v>117</v>
       </c>
@@ -1712,8 +1810,8 @@
       </c>
     </row>
     <row r="56" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
       <c r="D56" s="12" t="s">
         <v>120</v>
       </c>
@@ -1734,10 +1832,10 @@
       </c>
     </row>
     <row r="58" spans="2:5" ht="145" x14ac:dyDescent="0.35">
-      <c r="B58" s="16">
+      <c r="B58" s="24">
         <v>17</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="24" t="s">
         <v>123</v>
       </c>
       <c r="D58" s="8" t="s">
@@ -1748,8 +1846,8 @@
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
       <c r="D59" s="3" t="s">
         <v>129</v>
       </c>
@@ -1758,8 +1856,8 @@
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
       <c r="D60" s="8" t="s">
         <v>128</v>
       </c>
@@ -1768,16 +1866,16 @@
       </c>
     </row>
     <row r="61" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
       <c r="D61" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E61" s="2"/>
     </row>
     <row r="62" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
       <c r="D62" s="8" t="s">
         <v>132</v>
       </c>
@@ -1786,8 +1884,8 @@
       </c>
     </row>
     <row r="63" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
       <c r="D63" s="8" t="s">
         <v>134</v>
       </c>
@@ -1796,8 +1894,8 @@
       </c>
     </row>
     <row r="64" spans="2:5" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
       <c r="D64" s="8" t="s">
         <v>136</v>
       </c>
@@ -1806,8 +1904,8 @@
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="24"/>
       <c r="D65" s="8" t="s">
         <v>138</v>
       </c>
@@ -1816,8 +1914,8 @@
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
       <c r="D66" s="3" t="s">
         <v>141</v>
       </c>
@@ -1826,10 +1924,10 @@
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B67" s="13">
+      <c r="B67" s="14">
         <v>18</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="C67" s="17" t="s">
         <v>142</v>
       </c>
       <c r="D67" s="8" t="s">
@@ -1840,8 +1938,8 @@
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B68" s="14"/>
-      <c r="C68" s="23"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="18"/>
       <c r="D68" s="8" t="s">
         <v>146</v>
       </c>
@@ -1850,8 +1948,8 @@
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B69" s="14"/>
-      <c r="C69" s="23"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="18"/>
       <c r="D69" s="8" t="s">
         <v>147</v>
       </c>
@@ -1860,8 +1958,8 @@
       </c>
     </row>
     <row r="70" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B70" s="15"/>
-      <c r="C70" s="24"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="8" t="s">
         <v>150</v>
       </c>
@@ -1870,10 +1968,10 @@
       </c>
     </row>
     <row r="71" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B71" s="13">
+      <c r="B71" s="14">
         <v>19</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="14" t="s">
         <v>151</v>
       </c>
       <c r="D71" s="8" t="s">
@@ -1884,8 +1982,8 @@
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B72" s="15"/>
-      <c r="C72" s="15"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
       <c r="D72" s="8" t="s">
         <v>154</v>
       </c>
@@ -1921,74 +2019,189 @@
         <v>160</v>
       </c>
     </row>
-    <row r="75" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B75" s="2">
+    <row r="75" spans="2:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="B75" s="14">
         <v>22</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" t="s">
         <v>163</v>
       </c>
-      <c r="D75" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="E75" s="2"/>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="2"/>
+      <c r="E76" s="2" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="2"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="2"/>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="2"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="2"/>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="8"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B81" s="15"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="8" t="s">
+        <v>174</v>
+      </c>
       <c r="E81" s="2"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="2"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="2"/>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="2"/>
+      <c r="B83" s="15"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B84" s="15"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B85" s="15"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B86" s="15"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B87" s="15"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B89" s="14">
+        <v>23</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>192</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="33">
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="C58:C66"/>
+    <mergeCell ref="B58:B66"/>
+    <mergeCell ref="C75:C88"/>
+    <mergeCell ref="B75:B88"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C51:C56"/>
+    <mergeCell ref="B51:B56"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B67:B70"/>
     <mergeCell ref="C67:C70"/>
     <mergeCell ref="B71:B72"/>
@@ -2005,19 +2218,6 @@
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C51:C56"/>
-    <mergeCell ref="B51:B56"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C58:C66"/>
-    <mergeCell ref="B58:B66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>